<commit_message>
Redact raw UPF data from input datasets folder.
</commit_message>
<xml_diff>
--- a/Input data/Rigth-to-Food_Dataset_2024.xlsx
+++ b/Input data/Rigth-to-Food_Dataset_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate S\Dropbox\GitHub\FSCountdownIniative\FSCI 2024\Monitoring\Input Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate S\Dropbox\GitHub\FSCI_2024Interactions_Replication\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ABBBB1-CA70-44CF-9D8A-4D6B2F618B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408394BF-36F1-4B60-AE4F-96332A3251F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7AF86670-2164-4E94-8CDE-99E58814A19C}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="29040" windowHeight="15720" xr2:uid="{7AF86670-2164-4E94-8CDE-99E58814A19C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -554,10 +554,10 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Year added to FSCI data based on manual review of FAOLEX</t>
-  </si>
-  <si>
     <t>degree_of_recognition</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Rigth-to-Food_Dataset.xlsx]Sheet3!PivotTable2</c:name>
+    <c:name>[Rigth-to-Food_Dataset_2024.xlsx]Sheet3!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2935,7 +2935,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1C305C62-459D-44BA-B0C1-9F2FC2D31454}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Contitutional mechanism present">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1C305C62-459D-44BA-B0C1-9F2FC2D31454}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Contitutional mechanism present">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -3302,7 +3302,7 @@
   <dimension ref="A1:C310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3316,18 +3316,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>2023</v>
@@ -3335,10 +3335,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C3">
         <v>2023</v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>2023</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C5">
         <v>2023</v>
@@ -3368,10 +3368,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>2023</v>
@@ -3379,10 +3379,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C7">
         <v>2023</v>
@@ -3390,10 +3390,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <v>2023</v>
@@ -3401,10 +3401,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C9">
         <v>2023</v>
@@ -3412,10 +3412,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>2023</v>
@@ -3423,10 +3423,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C11">
         <v>2023</v>
@@ -3434,10 +3434,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>2023</v>
@@ -3445,10 +3445,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C13">
         <v>2023</v>
@@ -3456,10 +3456,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>2023</v>
@@ -3467,10 +3467,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>2023</v>
@@ -3478,10 +3478,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C16">
         <v>2023</v>
@@ -3489,10 +3489,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C17">
         <v>2023</v>
@@ -3500,10 +3500,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>2023</v>
@@ -3511,10 +3511,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C19">
         <v>2023</v>
@@ -3522,10 +3522,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C20">
         <v>2023</v>
@@ -3533,10 +3533,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>2023</v>
@@ -3544,10 +3544,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C22">
         <v>2023</v>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -3566,10 +3566,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C24">
         <v>2023</v>
@@ -3577,10 +3577,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C25">
         <v>2023</v>
@@ -3588,10 +3588,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>2023</v>
@@ -3599,10 +3599,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C27">
         <v>2023</v>
@@ -3610,10 +3610,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C28">
         <v>2023</v>
@@ -3621,10 +3621,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C29">
         <v>2023</v>
@@ -3632,10 +3632,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
       <c r="C30">
         <v>2023</v>
@@ -3643,10 +3643,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>2023</v>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C32">
         <v>2023</v>
@@ -3665,10 +3665,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C33">
         <v>2023</v>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -3687,10 +3687,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C35">
         <v>2023</v>
@@ -3698,10 +3698,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C36">
         <v>2023</v>
@@ -3709,10 +3709,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>2024</v>
@@ -3720,10 +3720,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>2023</v>
@@ -3731,10 +3731,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C39">
         <v>2023</v>
@@ -3742,10 +3742,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C40">
         <v>2023</v>
@@ -3753,10 +3753,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C41">
         <v>2023</v>
@@ -3764,10 +3764,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C42">
         <v>2023</v>
@@ -3775,10 +3775,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C43">
         <v>2023</v>
@@ -3786,10 +3786,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C44">
         <v>2023</v>
@@ -3797,10 +3797,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <v>2023</v>
@@ -3808,10 +3808,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C46">
         <v>2023</v>
@@ -3819,10 +3819,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C47">
         <v>2023</v>
@@ -3830,10 +3830,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C48">
         <v>2023</v>
@@ -3841,10 +3841,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C49">
         <v>2023</v>
@@ -3852,10 +3852,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C50">
         <v>2023</v>
@@ -3863,10 +3863,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C51">
         <v>2023</v>
@@ -3874,10 +3874,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C52">
         <v>2023</v>
@@ -3885,10 +3885,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C53">
         <v>2023</v>
@@ -3896,10 +3896,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C54">
         <v>2023</v>
@@ -3907,10 +3907,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>2023</v>
@@ -3918,10 +3918,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C56">
         <v>2023</v>
@@ -3929,10 +3929,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C57">
         <v>2023</v>
@@ -3940,10 +3940,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C58">
         <v>2023</v>
@@ -3951,10 +3951,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C59">
         <v>2023</v>
@@ -3962,10 +3962,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C60">
         <v>2023</v>
@@ -3973,10 +3973,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C61">
         <v>2023</v>
@@ -3984,10 +3984,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C62">
         <v>2023</v>
@@ -3995,10 +3995,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C63">
         <v>2023</v>
@@ -4006,10 +4006,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>2023</v>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C65">
         <v>2023</v>
@@ -4028,10 +4028,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C66">
         <v>2023</v>
@@ -4039,10 +4039,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C67">
         <v>2023</v>
@@ -4050,10 +4050,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C68">
         <v>2023</v>
@@ -4061,10 +4061,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C69">
         <v>2023</v>
@@ -4072,10 +4072,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="C70">
         <v>2023</v>
@@ -4083,10 +4083,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C71">
         <v>2023</v>
@@ -4094,10 +4094,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C72">
         <v>2023</v>
@@ -4105,10 +4105,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C73">
         <v>2023</v>
@@ -4116,10 +4116,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C74">
         <v>2023</v>
@@ -4127,10 +4127,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C75">
         <v>2023</v>
@@ -4138,10 +4138,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C76">
         <v>2023</v>
@@ -4149,10 +4149,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C77">
         <v>2023</v>
@@ -4160,7 +4160,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B78" t="s">
         <v>63</v>
@@ -4171,10 +4171,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C79">
         <v>2023</v>
@@ -4182,10 +4182,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C80">
         <v>2023</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
         <v>63</v>
@@ -4204,10 +4204,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C82">
         <v>2023</v>
@@ -4215,10 +4215,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C83">
         <v>2023</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
         <v>63</v>
@@ -4237,10 +4237,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C85">
         <v>2023</v>
@@ -4248,7 +4248,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
         <v>63</v>
@@ -4259,10 +4259,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C87">
         <v>2023</v>
@@ -4270,10 +4270,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C88">
         <v>2023</v>
@@ -4281,10 +4281,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C89">
         <v>2023</v>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s">
         <v>63</v>
@@ -4303,10 +4303,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C91">
         <v>2023</v>
@@ -4314,10 +4314,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C92">
         <v>2023</v>
@@ -4325,10 +4325,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C93">
         <v>2023</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="B94" t="s">
         <v>63</v>
@@ -4347,10 +4347,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="B95" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C95">
         <v>2023</v>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
         <v>63</v>
@@ -4369,10 +4369,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B97" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C97">
         <v>2023</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B98" t="s">
         <v>63</v>
@@ -4391,10 +4391,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C99">
         <v>2023</v>
@@ -4402,10 +4402,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="B100" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C100">
         <v>2023</v>
@@ -4413,7 +4413,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B101" t="s">
         <v>63</v>
@@ -4424,10 +4424,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="B102" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C102">
         <v>2023</v>
@@ -4435,10 +4435,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B103" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C103">
         <v>2023</v>
@@ -4446,10 +4446,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B104" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C104">
         <v>2023</v>
@@ -4457,7 +4457,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B105" t="s">
         <v>63</v>
@@ -4468,10 +4468,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C106">
         <v>2023</v>
@@ -4479,10 +4479,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B107" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C107">
         <v>2023</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B108" t="s">
         <v>63</v>
@@ -4501,10 +4501,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="B109" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C109">
         <v>2023</v>
@@ -4512,10 +4512,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C110">
         <v>2023</v>
@@ -4523,7 +4523,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B111" t="s">
         <v>63</v>
@@ -4534,10 +4534,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B112" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C112">
         <v>2023</v>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="B113" t="s">
         <v>63</v>
@@ -4556,10 +4556,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B114" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C114">
         <v>2023</v>
@@ -4567,7 +4567,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B115" t="s">
         <v>63</v>
@@ -4578,10 +4578,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B116" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C116">
         <v>2023</v>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B117" t="s">
         <v>63</v>
@@ -4600,10 +4600,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="B118" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C118">
         <v>2023</v>
@@ -4611,10 +4611,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C119">
         <v>2023</v>
@@ -4622,10 +4622,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C120">
         <v>2023</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="B121" t="s">
         <v>63</v>
@@ -4644,10 +4644,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C122">
         <v>2023</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B123" t="s">
         <v>63</v>
@@ -4666,10 +4666,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="B124" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C124">
         <v>2023</v>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B125" t="s">
         <v>63</v>
@@ -4691,7 +4691,7 @@
         <v>96</v>
       </c>
       <c r="B126" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C126">
         <v>2023</v>
@@ -4699,10 +4699,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B127" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C127">
         <v>2023</v>
@@ -4710,10 +4710,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C128">
         <v>2023</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="B129" t="s">
         <v>63</v>
@@ -4732,10 +4732,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B130" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C130">
         <v>2023</v>
@@ -4743,10 +4743,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C131">
         <v>2023</v>
@@ -4754,10 +4754,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B132" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C132">
         <v>2023</v>
@@ -4765,7 +4765,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="B133" t="s">
         <v>63</v>
@@ -4776,10 +4776,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B134" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C134">
         <v>2023</v>
@@ -4787,10 +4787,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C135">
         <v>2023</v>
@@ -4798,7 +4798,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B136" t="s">
         <v>63</v>
@@ -4809,10 +4809,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B137" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C137">
         <v>2023</v>
@@ -4820,10 +4820,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="B138" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C138">
         <v>2023</v>
@@ -4831,10 +4831,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="B139" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C139">
         <v>2023</v>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B140" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C140">
         <v>2023</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B141" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C141">
         <v>2023</v>
@@ -4864,10 +4864,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="B142" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C142">
         <v>2023</v>
@@ -4875,10 +4875,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="B143" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C143">
         <v>2023</v>
@@ -4886,10 +4886,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="B144" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C144">
         <v>2023</v>
@@ -4897,10 +4897,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C145">
         <v>2023</v>
@@ -4908,10 +4908,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="B146" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C146">
         <v>2023</v>
@@ -4919,7 +4919,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="B147" t="s">
         <v>63</v>
@@ -4930,7 +4930,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B148" t="s">
         <v>63</v>
@@ -4941,10 +4941,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B149" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C149">
         <v>2023</v>
@@ -4952,10 +4952,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B150" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C150">
         <v>2023</v>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="B151" t="s">
         <v>63</v>
@@ -4974,7 +4974,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="B152" t="s">
         <v>63</v>
@@ -4985,10 +4985,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="B153" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C153">
         <v>2023</v>
@@ -4996,10 +4996,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="B154" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C154">
         <v>2023</v>
@@ -5007,7 +5007,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="B155" t="s">
         <v>63</v>
@@ -5018,10 +5018,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="B156" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C156">
         <v>2023</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B157" t="s">
         <v>63</v>
@@ -5040,10 +5040,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="B158" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C158">
         <v>2023</v>
@@ -5051,7 +5051,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B159" t="s">
         <v>63</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B160" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C160">
         <v>2023</v>
@@ -5073,10 +5073,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="B161" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C161">
         <v>2023</v>
@@ -5084,10 +5084,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="B162" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C162">
         <v>2023</v>
@@ -5095,10 +5095,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>26</v>
+        <v>150</v>
       </c>
       <c r="B163" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C163">
         <v>2023</v>
@@ -5106,10 +5106,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="B164" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C164">
         <v>2023</v>
@@ -5117,10 +5117,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="B165" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C165">
         <v>2023</v>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B166" t="s">
         <v>63</v>
@@ -5139,10 +5139,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B167" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C167">
         <v>2023</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B168" t="s">
         <v>63</v>
@@ -5161,10 +5161,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="B169" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C169">
         <v>2023</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B170" t="s">
         <v>63</v>
@@ -5183,10 +5183,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="B171" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C171">
         <v>2023</v>
@@ -5194,10 +5194,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="B172" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C172">
         <v>2023</v>
@@ -5205,10 +5205,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>129</v>
+        <v>17</v>
       </c>
       <c r="B173" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C173">
         <v>2023</v>
@@ -5216,7 +5216,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B174" t="s">
         <v>63</v>
@@ -5227,10 +5227,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B175" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C175">
         <v>2023</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="B176" t="s">
         <v>63</v>
@@ -5249,7 +5249,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B177" t="s">
         <v>63</v>
@@ -5260,10 +5260,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="B178" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C178">
         <v>2023</v>
@@ -5271,7 +5271,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B179" t="s">
         <v>63</v>
@@ -5282,7 +5282,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="B180" t="s">
         <v>63</v>
@@ -5293,10 +5293,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B181" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C181">
         <v>2023</v>
@@ -5304,7 +5304,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B182" t="s">
         <v>63</v>
@@ -5315,10 +5315,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="B183" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C183">
         <v>2023</v>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B184" t="s">
         <v>63</v>
@@ -5337,10 +5337,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="B185" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C185">
         <v>2023</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="B186" t="s">
         <v>63</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="B187" t="s">
         <v>63</v>
@@ -5370,10 +5370,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="B188" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C188">
         <v>2023</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="B189" t="s">
         <v>136</v>
@@ -5392,10 +5392,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B190" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C190">
         <v>2023</v>
@@ -5403,10 +5403,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B191" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C191">
         <v>2023</v>
@@ -5414,10 +5414,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B192" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C192">
         <v>2023</v>
@@ -5425,10 +5425,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="B193" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C193">
         <v>2023</v>
@@ -5436,10 +5436,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B194" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C194">
         <v>2023</v>
@@ -5447,7 +5447,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="B195" t="s">
         <v>136</v>
@@ -5458,10 +5458,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="B196" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C196">
         <v>2023</v>
@@ -5469,7 +5469,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="B197" t="s">
         <v>136</v>
@@ -5480,10 +5480,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C198">
         <v>2023</v>
@@ -5491,10 +5491,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C199">
         <v>2023</v>
@@ -5502,10 +5502,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="B200" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C200">
         <v>2023</v>
@@ -5513,10 +5513,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C201">
         <v>2023</v>
@@ -5524,10 +5524,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B202" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C202">
         <v>2023</v>
@@ -5535,10 +5535,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B203" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C203">
         <v>2023</v>
@@ -5546,10 +5546,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B204" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C204">
         <v>2023</v>
@@ -5557,10 +5557,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B205" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C205">
         <v>2023</v>
@@ -5568,10 +5568,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="B206" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C206">
         <v>2023</v>
@@ -5579,7 +5579,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B207" t="s">
         <v>136</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="B208" t="s">
         <v>136</v>
@@ -5601,10 +5601,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B209" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C209">
         <v>2023</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B210" t="s">
         <v>136</v>
@@ -5623,10 +5623,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>139</v>
+        <v>55</v>
       </c>
       <c r="B211" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C211">
         <v>2023</v>
@@ -5634,10 +5634,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="B212" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C212">
         <v>2023</v>
@@ -5645,10 +5645,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B213" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C213">
         <v>2023</v>
@@ -5656,10 +5656,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="B214" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C214">
         <v>2023</v>
@@ -5667,10 +5667,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="B215" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C215">
         <v>2023</v>
@@ -5678,10 +5678,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B216" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C216">
         <v>2023</v>
@@ -5689,10 +5689,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B217" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C217">
         <v>2023</v>
@@ -5700,10 +5700,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="B218" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C218">
         <v>2023</v>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>141</v>
+        <v>24</v>
       </c>
       <c r="B219" t="s">
         <v>136</v>
@@ -5722,10 +5722,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="B220" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C220">
         <v>2023</v>
@@ -5733,10 +5733,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B221" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C221">
         <v>2023</v>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B222" t="s">
         <v>136</v>
@@ -5755,10 +5755,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="B223" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C223">
         <v>2023</v>
@@ -5766,7 +5766,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="B224" t="s">
         <v>136</v>
@@ -5777,10 +5777,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B225" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C225">
         <v>2023</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B226" t="s">
         <v>136</v>
@@ -5799,10 +5799,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="B227" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C227">
         <v>2023</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B228" t="s">
         <v>136</v>
@@ -5821,10 +5821,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B229" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C229">
         <v>2023</v>
@@ -5832,7 +5832,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="B230" t="s">
         <v>136</v>
@@ -5843,10 +5843,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B231" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C231">
         <v>2023</v>
@@ -5854,7 +5854,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B232" t="s">
         <v>136</v>
@@ -5865,10 +5865,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B233" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C233">
         <v>2023</v>
@@ -5876,10 +5876,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="B234" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C234">
         <v>2023</v>
@@ -5887,7 +5887,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="B235" t="s">
         <v>136</v>
@@ -5898,10 +5898,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="B236" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C236">
         <v>2023</v>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="B237" t="s">
         <v>136</v>
@@ -5920,10 +5920,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B238" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C238">
         <v>2023</v>
@@ -5931,7 +5931,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="B239" t="s">
         <v>136</v>
@@ -5942,10 +5942,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="B240" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C240">
         <v>2023</v>
@@ -5953,7 +5953,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="B241" t="s">
         <v>136</v>
@@ -5964,10 +5964,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B242" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C242">
         <v>2023</v>
@@ -5975,7 +5975,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B243" t="s">
         <v>136</v>
@@ -5986,10 +5986,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B244" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C244">
         <v>2023</v>
@@ -5997,7 +5997,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B245" t="s">
         <v>136</v>
@@ -6008,10 +6008,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="B246" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C246">
         <v>2023</v>
@@ -6019,7 +6019,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B247" t="s">
         <v>136</v>
@@ -6030,10 +6030,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B248" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C248">
         <v>2023</v>
@@ -6041,7 +6041,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="B249" t="s">
         <v>136</v>
@@ -6052,10 +6052,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B250" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C250">
         <v>2023</v>
@@ -6063,7 +6063,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="B251" t="s">
         <v>136</v>
@@ -6074,7 +6074,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B252" t="s">
         <v>136</v>
@@ -6085,10 +6085,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B253" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C253">
         <v>2023</v>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="B254" t="s">
         <v>136</v>
@@ -6107,10 +6107,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B255" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C255">
         <v>2023</v>
@@ -6118,7 +6118,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="B256" t="s">
         <v>136</v>
@@ -6129,10 +6129,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="B257" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C257">
         <v>2023</v>
@@ -6140,10 +6140,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B258" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C258">
         <v>2023</v>
@@ -6151,7 +6151,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="B259" t="s">
         <v>136</v>
@@ -6162,10 +6162,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="B260" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C260">
         <v>2023</v>
@@ -6173,10 +6173,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B261" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C261">
         <v>2023</v>
@@ -6184,7 +6184,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="B262" t="s">
         <v>136</v>
@@ -6195,10 +6195,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B263" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C263">
         <v>2023</v>
@@ -6206,7 +6206,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="B264" t="s">
         <v>136</v>
@@ -6217,10 +6217,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="B265" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C265">
         <v>2023</v>
@@ -6228,10 +6228,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B266" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C266">
         <v>2023</v>
@@ -6239,7 +6239,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
       <c r="B267" t="s">
         <v>136</v>
@@ -6250,10 +6250,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B268" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C268">
         <v>2023</v>
@@ -6261,7 +6261,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="B269" t="s">
         <v>136</v>
@@ -6272,7 +6272,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="B270" t="s">
         <v>136</v>
@@ -6283,10 +6283,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="B271" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C271">
         <v>2023</v>
@@ -6294,10 +6294,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="B272" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C272">
         <v>2023</v>
@@ -6305,10 +6305,10 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B273" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C273">
         <v>2023</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B274" t="s">
         <v>136</v>
@@ -6327,7 +6327,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="B275" t="s">
         <v>136</v>
@@ -6338,10 +6338,10 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B276" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C276">
         <v>2023</v>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="B277" t="s">
         <v>136</v>
@@ -6360,7 +6360,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="B278" t="s">
         <v>136</v>
@@ -6371,10 +6371,10 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B279" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C279">
         <v>2023</v>
@@ -6382,7 +6382,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B280" t="s">
         <v>136</v>
@@ -6393,10 +6393,10 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>127</v>
+        <v>42</v>
       </c>
       <c r="B281" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C281">
         <v>2023</v>
@@ -6404,10 +6404,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="B282" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C282">
         <v>2023</v>
@@ -6415,7 +6415,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="B283" t="s">
         <v>136</v>
@@ -6426,10 +6426,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>156</v>
+        <v>43</v>
       </c>
       <c r="B284" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C284">
         <v>2023</v>
@@ -6437,10 +6437,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B285" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C285">
         <v>2023</v>
@@ -6448,7 +6448,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B286" t="s">
         <v>136</v>
@@ -6459,10 +6459,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B287" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C287">
         <v>2023</v>
@@ -6470,7 +6470,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B288" t="s">
         <v>136</v>
@@ -6481,10 +6481,10 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="B289" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C289">
         <v>2023</v>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B290" t="s">
         <v>136</v>
@@ -6503,7 +6503,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>41</v>
+        <v>160</v>
       </c>
       <c r="B291" t="s">
         <v>136</v>
@@ -6514,10 +6514,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>158</v>
+        <v>59</v>
       </c>
       <c r="B292" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C292">
         <v>2023</v>
@@ -6525,7 +6525,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="B293" t="s">
         <v>136</v>
@@ -6536,10 +6536,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="B294" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C294">
         <v>2023</v>
@@ -6547,10 +6547,10 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>133</v>
+        <v>29</v>
       </c>
       <c r="B295" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C295">
         <v>2023</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B296" t="s">
         <v>136</v>
@@ -6569,7 +6569,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="B297" t="s">
         <v>136</v>
@@ -6580,10 +6580,10 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="B298" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C298">
         <v>2023</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="B299" t="s">
         <v>136</v>
@@ -6602,7 +6602,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B300" t="s">
         <v>136</v>
@@ -6613,10 +6613,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B301" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C301">
         <v>2023</v>
@@ -6624,10 +6624,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B302" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C302">
         <v>2023</v>
@@ -6635,7 +6635,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
       <c r="B303" t="s">
         <v>136</v>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B304" t="s">
         <v>136</v>
@@ -6657,7 +6657,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B305" t="s">
         <v>136</v>
@@ -6668,7 +6668,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="B306" t="s">
         <v>136</v>
@@ -6679,10 +6679,10 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="B307" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="C307">
         <v>2023</v>
@@ -6690,10 +6690,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>165</v>
+        <v>30</v>
       </c>
       <c r="B308" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="C308">
         <v>2023</v>
@@ -6701,10 +6701,10 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="B309" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C309">
         <v>2023</v>
@@ -6722,7 +6722,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B310" xr:uid="{1F1B3A89-4930-444F-AB01-4CC0323E40D6}"/>
+  <autoFilter ref="A1:B310" xr:uid="{1F1B3A89-4930-444F-AB01-4CC0323E40D6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B310">
+      <sortCondition ref="A1:A310"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>